<commit_message>
more accurate abs/relative abundance in MARGO now
I manually label the species data type (as 1,2,3) [last commit],
with comments in related scripts.
Also change the code and manually check the output.
</commit_message>
<xml_diff>
--- a/raw/MARGO/clean format/LGM_MARGO_Pacific.xlsx
+++ b/raw/MARGO/clean format/LGM_MARGO_Pacific.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yingrui/Science/lgm_foram_census/raw/MARGO/clean format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{60DEAC2E-48AE-DE46-A73A-294F3A4CB328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE07457F-1CFB-3B45-8784-2EEABC25B188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LGM_MARGO_Pacific" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1323,11 +1323,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AP2" sqref="AP2"/>
+    <sheetView tabSelected="1" topLeftCell="P99" workbookViewId="0">
+      <selection activeCell="AP117" sqref="AP117:AP133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16154,7 +16154,7 @@
         <v>309</v>
       </c>
       <c r="AP116">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:42" x14ac:dyDescent="0.2">
@@ -16279,7 +16279,7 @@
         <v>365</v>
       </c>
       <c r="AP117">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:42" x14ac:dyDescent="0.2">
@@ -16404,7 +16404,7 @@
         <v>394</v>
       </c>
       <c r="AP118">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:42" x14ac:dyDescent="0.2">
@@ -16529,7 +16529,7 @@
         <v>380</v>
       </c>
       <c r="AP119">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:42" x14ac:dyDescent="0.2">
@@ -16654,7 +16654,7 @@
         <v>422</v>
       </c>
       <c r="AP120">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:42" x14ac:dyDescent="0.2">
@@ -16779,7 +16779,7 @@
         <v>325</v>
       </c>
       <c r="AP121">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:42" x14ac:dyDescent="0.2">
@@ -16904,7 +16904,7 @@
         <v>393</v>
       </c>
       <c r="AP122">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:42" x14ac:dyDescent="0.2">
@@ -17029,7 +17029,7 @@
         <v>358</v>
       </c>
       <c r="AP123">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:42" x14ac:dyDescent="0.2">
@@ -17154,7 +17154,7 @@
         <v>331</v>
       </c>
       <c r="AP124">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:42" x14ac:dyDescent="0.2">
@@ -17279,7 +17279,7 @@
         <v>1271</v>
       </c>
       <c r="AP125">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:42" x14ac:dyDescent="0.2">
@@ -17404,7 +17404,7 @@
         <v>367</v>
       </c>
       <c r="AP126">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:42" x14ac:dyDescent="0.2">
@@ -17529,7 +17529,7 @@
         <v>442</v>
       </c>
       <c r="AP127">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:42" x14ac:dyDescent="0.2">
@@ -17654,7 +17654,7 @@
         <v>443</v>
       </c>
       <c r="AP128">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:42" x14ac:dyDescent="0.2">
@@ -17779,7 +17779,7 @@
         <v>366</v>
       </c>
       <c r="AP129">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:42" x14ac:dyDescent="0.2">
@@ -17904,7 +17904,7 @@
         <v>420</v>
       </c>
       <c r="AP130">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:42" x14ac:dyDescent="0.2">
@@ -18029,7 +18029,7 @@
         <v>455</v>
       </c>
       <c r="AP131">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:42" x14ac:dyDescent="0.2">
@@ -18154,7 +18154,7 @@
         <v>445</v>
       </c>
       <c r="AP132">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:42" x14ac:dyDescent="0.2">
@@ -18279,7 +18279,7 @@
         <v>1155</v>
       </c>
       <c r="AP133">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:42" x14ac:dyDescent="0.2">

</xml_diff>